<commit_message>
adding sheet with sequencing data
</commit_message>
<xml_diff>
--- a/examples/ex02_Amersfoort/amersfoort.xlsx
+++ b/examples/ex02_Amersfoort/amersfoort.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="environment" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="contaminants" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="metabolites" sheetId="3" state="visible" r:id="rId5"/>
     <sheet name="isotopes" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="sequencing" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="430">
   <si>
     <t xml:space="preserve">sample_name</t>
   </si>
@@ -1287,6 +1288,33 @@
   <si>
     <t xml:space="preserve">O7_t4</t>
   </si>
+  <si>
+    <t xml:space="preserve">sample_nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total bacteria 16SRrna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzene carboxylase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NirS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NarG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BssA SRB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BssA nitraat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peptococcus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nr</t>
+  </si>
 </sst>
 </file>
 
@@ -1295,7 +1323,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1316,6 +1344,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1360,7 +1395,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1371,6 +1406,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1499,7 +1542,7 @@
   <dimension ref="A1:X35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4104,8 +4147,8 @@
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7263,7 +7306,7 @@
   <dimension ref="A1:MM34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="ML1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="MS15" activeCellId="0" sqref="MS15"/>
+      <selection pane="topLeft" activeCell="MS15" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7288,7 +7331,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="84.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="1" width="84.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="59" style="1" width="84.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="62" style="1" width="58.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="62" style="1" width="58.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="1" width="59.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="1" width="59.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="73" style="1" width="59.65"/>
@@ -7300,7 +7343,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="1" width="84.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="101" min="101" style="1" width="84.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="102" style="1" width="84.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="105" style="1" width="58.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="113" min="105" style="1" width="58.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="114" style="1" width="59.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="1" width="59.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="116" style="1" width="59.65"/>
@@ -7309,7 +7352,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="126" style="1" width="49.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="135" min="135" style="1" width="50.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="137" min="136" style="1" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="138" style="1" width="29.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="146" min="138" style="1" width="29.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="147" min="147" style="1" width="30.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="148" min="148" style="1" width="30.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="149" min="149" style="1" width="20.45"/>
@@ -7337,15 +7380,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="217" min="217" style="1" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="218" min="218" style="1" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="222" min="219" style="1" width="26.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="223" min="223" style="1" width="7.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="223" min="223" style="1" width="7.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="228" min="224" style="1" width="42.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="234" min="229" style="1" width="57.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="238" min="235" style="1" width="39.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="242" min="239" style="1" width="24.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="243" style="1" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="246" min="243" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="247" min="247" style="1" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="248" min="248" style="1" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="249" style="1" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="249" min="249" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="250" min="250" style="1" width="10.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="252" min="251" style="1" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="253" min="253" style="1" width="48.11"/>
@@ -43275,7 +43318,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -43289,7 +43332,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="20.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="1" width="27.12"/>
@@ -46348,4 +46391,953 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L35"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="1" width="10.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>799641.666666667</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>336666.666666667</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>23000</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>8539.9459950898</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>726.223090159482</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>8071.60528751054</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>466842.00336629</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>893.381040991093</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>34533.1861529799</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>7182.00062363653</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>15351.6323054694</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>508222.439292535</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>25710.9141782482</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1527.6979003397</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1367.03165065601</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>2228.26488988377</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>34140.9144951505</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>12270.2595609119</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>86025.3634827033</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>11366.2241228162</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>56926.9382175487</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>8371218.04435184</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>315356.459796759</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>178014.672181414</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>51568.4528720404</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>4878382.85432252</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>11849.0826105995</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>1992.53947044613</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>32393.9369571992</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1.28723526569743</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>24436.2309270047</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>18433.5597935386</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>350807.911118742</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>83773.1829990723</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>17185.2539296265</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>6098.56027790906</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>3877.592130143</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>289747.844651168</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>183.864203895326</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>745.791427783727</v>
+      </c>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>32950</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>79333.3333333333</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <v>9783.33333333333</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>18833.3333333333</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>104391.666666667</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>57.2974234247097</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <v>60833.3333333333</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <v>4408.88888888889</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>8590</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>4095</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>4.10706662063471</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>87750</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>9.7858742455594</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>54333.3333333333</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>4304.16666666667</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>640500</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>11816.6666666667</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>5860</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>45068750</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>2.64106708402929</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <v>304166.666666667</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <v>711078.125</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>260.0625</v>
+      </c>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>31001.8638455069</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>20.1202381291977</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>78.9992264836742</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <v>654.655669599332</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>106838.668934382</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>90.6043587158942</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>1057.94728429677</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>133352.253106746</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>63287.3155373967</v>
+      </c>
+      <c r="E18" s="1" t="n">
+        <v>165728.715837796</v>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>2332803.44625201</v>
+      </c>
+      <c r="G18" s="1" t="n">
+        <v>75455.9456091021</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>15706.9457476502</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>32.8652272092314</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>428.811694125426</v>
+      </c>
+      <c r="E19" s="1" t="n">
+        <v>627.782788747258</v>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>89358.478850588</v>
+      </c>
+      <c r="G19" s="1" t="n">
+        <v>220.186362740821</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>601.682883399349</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>164672.976093138</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>319.469761117067</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>3827.11706825075</v>
+      </c>
+      <c r="E20" s="1" t="n">
+        <v>8182.86434773892</v>
+      </c>
+      <c r="F20" s="1" t="n">
+        <v>1295277.8312389</v>
+      </c>
+      <c r="G20" s="1" t="n">
+        <v>14480.6129174977</v>
+      </c>
+      <c r="H20" s="1" t="n">
+        <v>3331.77644565305</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>135500.094595913</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>2.51239259867797</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>365955.727430726</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <v>49148.12597431</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <v>4373106.20734064</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <v>1204088.91548226</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <v>50.2622457480147</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>338.055043358053</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <v>121.388320779765</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <v>240.708433852132</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>6857.08807814433</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <v>4128.40094660801</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <v>3045.9317853488</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <v>33698.7641688257</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <v>82059.2055506272</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <v>55.8118729450187</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>2524.37366661602</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>160.161918270151</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <v>487.097893957527</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <v>1012.56469148518</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>15857.3247530278</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <v>1134.43210122714</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>1049.61196309574</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>12782.438801812</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>2380.78827755999</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>722.568060009517</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>1254.35783696339</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>643570.474675248</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>976.032656628373</v>
+      </c>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>3046.51802095853</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>1677.77275226295</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>1079.95316777295</v>
+      </c>
+      <c r="F27" s="1" t="n">
+        <v>145850.256086035</v>
+      </c>
+      <c r="G27" s="1" t="n">
+        <v>4604.25209755172</v>
+      </c>
+      <c r="H27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>3158.02526537885</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <v>5076.0314509884</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>4046.68809793535</v>
+      </c>
+      <c r="F28" s="1" t="n">
+        <v>310638.881125958</v>
+      </c>
+      <c r="G28" s="1" t="n">
+        <v>7899.45366254307</v>
+      </c>
+      <c r="H28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>10837.8445559295</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <v>5263.8367250768</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>2276.5375275143</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>178812.668909704</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>12625</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>91.005063294962</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>3416.66666666667</v>
+      </c>
+      <c r="F30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>43825.8509466303</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>222.105930077391</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>3023.46405469856</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>3135.34209116679</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>414689.030994863</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>3881.35975274414</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>112.413642505767</v>
+      </c>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>6761.83085409313</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>1665.73313389372</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>4720.23663494565</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>277494.480673486</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>113833.333333333</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>67000</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>2033.33333333333</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>138108.333333333</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="n">
+        <v>35316.6666666667</v>
+      </c>
+      <c r="F34" s="1" t="n">
+        <v>16260</v>
+      </c>
+      <c r="G34" s="1" t="n">
+        <v>2050</v>
+      </c>
+      <c r="H34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>1197.05128254705</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <v>580.85383533419</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <v>381.006251776828</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <v>18975.6127484183</v>
+      </c>
+      <c r="G35" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>